<commit_message>
[FIX] #1510 delete column bal-debit, credit in trial balance
</commit_message>
<xml_diff>
--- a/cmo_trial_balance_extension/xlsx_template/trial_balance.xlsx
+++ b/cmo_trial_balance_extension/xlsx_template/trial_balance.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Trial Balance for CMO</t>
   </si>
@@ -44,12 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">Moving – Credit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moving Bal – Debit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moving Bal – Credit</t>
   </si>
   <si>
     <t xml:space="preserve">Current Bal – Debit</t>
@@ -318,9 +312,10 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="23.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="3" width="20.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="11" style="2" width="34.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="3" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="9" style="2" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1021" style="0" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="25.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -334,8 +329,8 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
@@ -348,8 +343,8 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
@@ -1360,8 +1355,6 @@
       <c r="AMD2" s="0"/>
       <c r="AME2" s="0"/>
       <c r="AMF2" s="0"/>
-      <c r="AMG2" s="0"/>
-      <c r="AMH2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
@@ -1374,8 +1367,8 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
@@ -2386,8 +2379,6 @@
       <c r="AMD3" s="0"/>
       <c r="AME3" s="0"/>
       <c r="AMF3" s="0"/>
-      <c r="AMG3" s="0"/>
-      <c r="AMH3" s="0"/>
     </row>
     <row r="4" s="10" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0"/>
@@ -2398,8 +2389,8 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="ALD4" s="2"/>
+      <c r="ALE4" s="2"/>
       <c r="ALF4" s="2"/>
       <c r="ALG4" s="2"/>
       <c r="ALH4" s="2"/>
@@ -2427,8 +2418,8 @@
       <c r="AMD4" s="2"/>
       <c r="AME4" s="2"/>
       <c r="AMF4" s="2"/>
-      <c r="AMG4" s="2"/>
-      <c r="AMH4" s="2"/>
+      <c r="AMG4" s="0"/>
+      <c r="AMH4" s="0"/>
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
@@ -2451,17 +2442,11 @@
       <c r="F5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>